<commit_message>
chg: added placeholder for range 8
</commit_message>
<xml_diff>
--- a/COMMUNICATION/TRMT Frequency and Callsign master list.xlsx
+++ b/COMMUNICATION/TRMT Frequency and Callsign master list.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="944">
   <si>
     <t>AWACS</t>
   </si>
@@ -2886,6 +2886,15 @@
   </si>
   <si>
     <t>VHG</t>
+  </si>
+  <si>
+    <t>Gazipasa?</t>
+  </si>
+  <si>
+    <t>Akratori</t>
+  </si>
+  <si>
+    <t>Sanliurfa</t>
   </si>
 </sst>
 </file>
@@ -4403,6 +4412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4643,7 +4653,6 @@
     <xf numFmtId="0" fontId="25" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4772,6 +4781,110 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>179917</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8604250" y="1841500"/>
+          <a:ext cx="5638800" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8658225" y="857250"/>
+          <a:ext cx="5638800" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5283,11 +5396,11 @@
       </c>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
-      <c r="S3" s="210" t="s">
+      <c r="S3" s="211" t="s">
         <v>282</v>
       </c>
-      <c r="T3" s="210"/>
-      <c r="U3" s="210"/>
+      <c r="T3" s="211"/>
+      <c r="U3" s="211"/>
       <c r="W3" s="7" t="s">
         <v>2</v>
       </c>
@@ -5298,13 +5411,13 @@
         <v>479</v>
       </c>
       <c r="Z3" s="120"/>
-      <c r="AD3" s="212" t="s">
+      <c r="AD3" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="213"/>
-      <c r="AF3" s="213"/>
-      <c r="AG3" s="213"/>
-      <c r="AH3" s="214"/>
+      <c r="AE3" s="214"/>
+      <c r="AF3" s="214"/>
+      <c r="AG3" s="214"/>
+      <c r="AH3" s="215"/>
     </row>
     <row r="4" spans="2:34" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -5350,7 +5463,7 @@
         <v>10</v>
       </c>
       <c r="P4" s="52"/>
-      <c r="S4" s="215" t="s">
+      <c r="S4" s="216" t="s">
         <v>636</v>
       </c>
       <c r="T4" s="97" t="s">
@@ -5421,7 +5534,7 @@
         <v>22</v>
       </c>
       <c r="P5" s="52"/>
-      <c r="S5" s="216"/>
+      <c r="S5" s="217"/>
       <c r="T5" s="31" t="s">
         <v>605</v>
       </c>
@@ -5438,7 +5551,7 @@
         <v>487</v>
       </c>
       <c r="Z5" s="120"/>
-      <c r="AB5" s="289"/>
+      <c r="AB5" s="209"/>
       <c r="AD5" s="7" t="s">
         <v>492</v>
       </c>
@@ -5501,7 +5614,7 @@
         <v>654</v>
       </c>
       <c r="R6" s="3"/>
-      <c r="S6" s="217"/>
+      <c r="S6" s="218"/>
       <c r="T6" s="99" t="s">
         <v>638</v>
       </c>
@@ -5583,7 +5696,7 @@
         <v>284</v>
       </c>
       <c r="R7" s="3"/>
-      <c r="S7" s="215" t="s">
+      <c r="S7" s="216" t="s">
         <v>642</v>
       </c>
       <c r="T7" s="97" t="s">
@@ -5664,7 +5777,7 @@
         <v>285</v>
       </c>
       <c r="R8" s="3"/>
-      <c r="S8" s="216"/>
+      <c r="S8" s="217"/>
       <c r="T8" s="31" t="s">
         <v>605</v>
       </c>
@@ -5733,7 +5846,7 @@
         <v>286</v>
       </c>
       <c r="R9" s="3"/>
-      <c r="S9" s="217"/>
+      <c r="S9" s="218"/>
       <c r="T9" s="99" t="s">
         <v>638</v>
       </c>
@@ -5878,7 +5991,7 @@
         <v>9</v>
       </c>
       <c r="R11" s="3"/>
-      <c r="S11" s="219" t="s">
+      <c r="S11" s="220" t="s">
         <v>643</v>
       </c>
       <c r="T11" s="102" t="s">
@@ -5954,7 +6067,7 @@
       <c r="P12" s="93"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="220"/>
+      <c r="S12" s="221"/>
       <c r="T12" s="96" t="s">
         <v>605</v>
       </c>
@@ -6025,7 +6138,7 @@
       <c r="P13" s="93"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="221"/>
+      <c r="S13" s="222"/>
       <c r="T13" s="104" t="s">
         <v>638</v>
       </c>
@@ -6050,11 +6163,11 @@
       <c r="AC13" t="s">
         <v>34</v>
       </c>
-      <c r="AE13" s="212" t="s">
+      <c r="AE13" s="213" t="s">
         <v>628</v>
       </c>
-      <c r="AF13" s="213"/>
-      <c r="AG13" s="214"/>
+      <c r="AF13" s="214"/>
+      <c r="AG13" s="215"/>
     </row>
     <row r="14" spans="2:34" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -6102,7 +6215,7 @@
         <v>281</v>
       </c>
       <c r="R14" s="3"/>
-      <c r="S14" s="215" t="s">
+      <c r="S14" s="216" t="s">
         <v>646</v>
       </c>
       <c r="T14" s="102" t="s">
@@ -6169,22 +6282,22 @@
         <v>294</v>
       </c>
       <c r="R15" s="3"/>
-      <c r="S15" s="216"/>
+      <c r="S15" s="217"/>
       <c r="T15" s="96" t="s">
         <v>605</v>
       </c>
       <c r="U15" s="21" t="s">
         <v>648</v>
       </c>
-      <c r="W15" s="211" t="s">
+      <c r="W15" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="X15" s="211"/>
-      <c r="Y15" s="211"/>
-      <c r="Z15" s="211"/>
-      <c r="AA15" s="211"/>
-      <c r="AB15" s="211"/>
-      <c r="AC15" s="211"/>
+      <c r="X15" s="212"/>
+      <c r="Y15" s="212"/>
+      <c r="Z15" s="212"/>
+      <c r="AA15" s="212"/>
+      <c r="AB15" s="212"/>
+      <c r="AC15" s="212"/>
       <c r="AE15" s="7" t="s">
         <v>620</v>
       </c>
@@ -6240,7 +6353,7 @@
         <v>293</v>
       </c>
       <c r="R16" s="3"/>
-      <c r="S16" s="217"/>
+      <c r="S16" s="218"/>
       <c r="T16" s="104" t="s">
         <v>638</v>
       </c>
@@ -6577,11 +6690,11 @@
         <v>302</v>
       </c>
       <c r="R20" s="3"/>
-      <c r="S20" s="211" t="s">
+      <c r="S20" s="212" t="s">
         <v>281</v>
       </c>
-      <c r="T20" s="211"/>
-      <c r="U20" s="211"/>
+      <c r="T20" s="212"/>
+      <c r="U20" s="212"/>
       <c r="V20" s="3"/>
       <c r="W20" s="39" t="s">
         <v>907</v>
@@ -7308,34 +7421,34 @@
       </c>
     </row>
     <row r="32" spans="2:34">
-      <c r="B32" s="212" t="s">
+      <c r="B32" s="213" t="s">
         <v>299</v>
       </c>
-      <c r="C32" s="213"/>
-      <c r="D32" s="213"/>
-      <c r="E32" s="213"/>
-      <c r="F32" s="213"/>
-      <c r="G32" s="213"/>
-      <c r="H32" s="214"/>
-      <c r="J32" s="211" t="s">
+      <c r="C32" s="214"/>
+      <c r="D32" s="214"/>
+      <c r="E32" s="214"/>
+      <c r="F32" s="214"/>
+      <c r="G32" s="214"/>
+      <c r="H32" s="215"/>
+      <c r="J32" s="212" t="s">
         <v>300</v>
       </c>
-      <c r="K32" s="211"/>
-      <c r="L32" s="211"/>
-      <c r="M32" s="211"/>
-      <c r="N32" s="211"/>
-      <c r="O32" s="211"/>
-      <c r="P32" s="211"/>
-      <c r="Q32" s="211"/>
-      <c r="U32" s="211" t="s">
+      <c r="K32" s="212"/>
+      <c r="L32" s="212"/>
+      <c r="M32" s="212"/>
+      <c r="N32" s="212"/>
+      <c r="O32" s="212"/>
+      <c r="P32" s="212"/>
+      <c r="Q32" s="212"/>
+      <c r="U32" s="212" t="s">
         <v>283</v>
       </c>
-      <c r="V32" s="211"/>
-      <c r="W32" s="211"/>
-      <c r="X32" s="211"/>
-      <c r="Y32" s="211"/>
-      <c r="Z32" s="211"/>
-      <c r="AA32" s="211"/>
+      <c r="V32" s="212"/>
+      <c r="W32" s="212"/>
+      <c r="X32" s="212"/>
+      <c r="Y32" s="212"/>
+      <c r="Z32" s="212"/>
+      <c r="AA32" s="212"/>
     </row>
     <row r="33" spans="2:37">
       <c r="B33" s="51" t="s">
@@ -7618,7 +7731,7 @@
       <c r="AA36" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="AE36" s="209" t="s">
+      <c r="AE36" s="210" t="s">
         <v>694</v>
       </c>
       <c r="AF36" s="7" t="s">
@@ -7704,7 +7817,7 @@
       <c r="AA37" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AE37" s="209"/>
+      <c r="AE37" s="210"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
       <c r="AH37" s="7"/>
@@ -7776,7 +7889,7 @@
       <c r="AA38" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AE38" s="209"/>
+      <c r="AE38" s="210"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
       <c r="AH38" s="7"/>
@@ -7833,7 +7946,7 @@
       <c r="AA39" s="7" t="s">
         <v>594</v>
       </c>
-      <c r="AE39" s="209"/>
+      <c r="AE39" s="210"/>
       <c r="AF39" s="7"/>
       <c r="AG39" s="7"/>
       <c r="AH39" s="7"/>
@@ -7848,16 +7961,16 @@
       <c r="F40" t="s">
         <v>566</v>
       </c>
-      <c r="J40" s="218" t="s">
+      <c r="J40" s="219" t="s">
         <v>475</v>
       </c>
-      <c r="K40" s="218"/>
-      <c r="L40" s="218"/>
-      <c r="M40" s="218"/>
-      <c r="N40" s="218"/>
-      <c r="O40" s="218"/>
-      <c r="P40" s="218"/>
-      <c r="Q40" s="218"/>
+      <c r="K40" s="219"/>
+      <c r="L40" s="219"/>
+      <c r="M40" s="219"/>
+      <c r="N40" s="219"/>
+      <c r="O40" s="219"/>
+      <c r="P40" s="219"/>
+      <c r="Q40" s="219"/>
       <c r="T40">
         <v>7</v>
       </c>
@@ -8326,34 +8439,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="273" t="s">
+      <c r="A1" s="274" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="273"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="274"/>
-      <c r="B2" s="274"/>
-      <c r="C2" s="274"/>
-      <c r="D2" s="274"/>
-      <c r="E2" s="274"/>
-      <c r="F2" s="274"/>
+      <c r="A2" s="275"/>
+      <c r="B2" s="275"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="235"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="234" t="s">
+      <c r="B3" s="236"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="235" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="235"/>
-      <c r="F3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="237"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -8710,14 +8823,14 @@
       <c r="F21" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="N21" s="275" t="s">
+      <c r="N21" s="276" t="s">
         <v>821</v>
       </c>
-      <c r="O21" s="275"/>
-      <c r="P21" s="275"/>
-      <c r="Q21" s="275"/>
-      <c r="R21" s="275"/>
-      <c r="S21" s="275"/>
+      <c r="O21" s="276"/>
+      <c r="P21" s="276"/>
+      <c r="Q21" s="276"/>
+      <c r="R21" s="276"/>
+      <c r="S21" s="276"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1">
       <c r="A22" s="54">
@@ -8738,12 +8851,12 @@
       <c r="F22" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="O22" s="276" t="s">
+      <c r="O22" s="277" t="s">
         <v>363</v>
       </c>
-      <c r="P22" s="276"/>
-      <c r="Q22" s="276"/>
-      <c r="R22" s="276"/>
+      <c r="P22" s="277"/>
+      <c r="Q22" s="277"/>
+      <c r="R22" s="277"/>
     </row>
     <row r="23" spans="1:19" ht="19.5" thickBot="1">
       <c r="A23" s="54">
@@ -9000,22 +9113,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="276" t="s">
         <v>821</v>
       </c>
-      <c r="B1" s="275"/>
-      <c r="C1" s="275"/>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="275"/>
+      <c r="B1" s="276"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="276" t="s">
+      <c r="B2" s="277" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="276"/>
-      <c r="D2" s="276"/>
-      <c r="E2" s="276"/>
+      <c r="C2" s="277"/>
+      <c r="D2" s="277"/>
+      <c r="E2" s="277"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -10769,40 +10882,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="283" t="s">
+      <c r="A1" s="284" t="s">
         <v>886</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="284"/>
-      <c r="G1" s="284"/>
-      <c r="H1" s="285"/>
+      <c r="B1" s="285"/>
+      <c r="C1" s="285"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="286"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="286"/>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287"/>
-      <c r="H2" s="288"/>
+      <c r="A2" s="287"/>
+      <c r="B2" s="288"/>
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288"/>
+      <c r="H2" s="289"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="278" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="278"/>
-      <c r="C3" s="278"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="277" t="s">
+      <c r="B3" s="279"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="278" t="s">
         <v>841</v>
       </c>
-      <c r="F3" s="278"/>
-      <c r="G3" s="278"/>
-      <c r="H3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="280"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="177">
@@ -11121,18 +11234,18 @@
       <c r="H21" s="169"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="280" t="s">
+      <c r="A22" s="281" t="s">
         <v>842</v>
       </c>
-      <c r="B22" s="281"/>
-      <c r="C22" s="281"/>
-      <c r="D22" s="282"/>
-      <c r="E22" s="280" t="s">
+      <c r="B22" s="282"/>
+      <c r="C22" s="282"/>
+      <c r="D22" s="283"/>
+      <c r="E22" s="281" t="s">
         <v>843</v>
       </c>
-      <c r="F22" s="281"/>
-      <c r="G22" s="281"/>
-      <c r="H22" s="282"/>
+      <c r="F22" s="282"/>
+      <c r="G22" s="282"/>
+      <c r="H22" s="283"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="160">
@@ -11523,40 +11636,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="222" t="s">
+      <c r="A1" s="223" t="s">
         <v>892</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="224"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
+      <c r="G1" s="224"/>
+      <c r="H1" s="225"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="225"/>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="227"/>
+      <c r="A2" s="226"/>
+      <c r="B2" s="227"/>
+      <c r="C2" s="227"/>
+      <c r="D2" s="227"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="227"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="228"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="229" t="s">
         <v>606</v>
       </c>
-      <c r="B3" s="229"/>
-      <c r="C3" s="229"/>
-      <c r="D3" s="229"/>
-      <c r="E3" s="229" t="s">
+      <c r="B3" s="230"/>
+      <c r="C3" s="230"/>
+      <c r="D3" s="230"/>
+      <c r="E3" s="230" t="s">
         <v>607</v>
       </c>
-      <c r="F3" s="229"/>
-      <c r="G3" s="229"/>
-      <c r="H3" s="230"/>
+      <c r="F3" s="230"/>
+      <c r="G3" s="230"/>
+      <c r="H3" s="231"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" thickBot="1">
       <c r="A4" s="77">
@@ -11653,6 +11766,9 @@
       <c r="H7" s="79" t="s">
         <v>643</v>
       </c>
+      <c r="I7" t="s">
+        <v>941</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" thickBot="1">
       <c r="A8" s="77">
@@ -12026,6 +12142,9 @@
       <c r="F21" s="79"/>
       <c r="G21" s="80"/>
       <c r="H21" s="79"/>
+      <c r="I21" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="18.75" thickBot="1">
       <c r="A22" s="77">
@@ -12046,6 +12165,9 @@
       <c r="F22" s="79"/>
       <c r="G22" s="80"/>
       <c r="H22" s="79"/>
+      <c r="I22" t="s">
+        <v>943</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="18.75" thickBot="1">
       <c r="A23" s="77">
@@ -12610,14 +12732,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="233"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="234"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -12628,16 +12750,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="235"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="234" t="s">
+      <c r="B3" s="236"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="235" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="235"/>
-      <c r="F3" s="236"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="237"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -12907,28 +13029,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="241" t="s">
         <v>891</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="238" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="239"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="240"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -13203,16 +13325,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="238" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
-      <c r="E15" s="238"/>
-      <c r="F15" s="238"/>
-      <c r="G15" s="238"/>
-      <c r="H15" s="239"/>
+      <c r="B15" s="239"/>
+      <c r="C15" s="239"/>
+      <c r="D15" s="239"/>
+      <c r="E15" s="239"/>
+      <c r="F15" s="239"/>
+      <c r="G15" s="239"/>
+      <c r="H15" s="240"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -13502,16 +13624,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="237" t="s">
+      <c r="A28" s="238" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="238"/>
-      <c r="C28" s="238"/>
-      <c r="D28" s="238"/>
-      <c r="E28" s="238"/>
-      <c r="F28" s="238"/>
-      <c r="G28" s="238"/>
-      <c r="H28" s="239"/>
+      <c r="B28" s="239"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="239"/>
+      <c r="E28" s="239"/>
+      <c r="F28" s="239"/>
+      <c r="G28" s="239"/>
+      <c r="H28" s="240"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -13824,12 +13946,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="242" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -14037,28 +14159,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="242" t="s">
+      <c r="A1" s="243" t="s">
         <v>889</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="243"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="238" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="239"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="240"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -14349,12 +14471,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="238" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="239"/>
+      <c r="B15" s="239"/>
+      <c r="C15" s="239"/>
+      <c r="D15" s="240"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -14522,12 +14644,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="237" t="s">
+      <c r="A28" s="238" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="238"/>
-      <c r="C28" s="238"/>
-      <c r="D28" s="239"/>
+      <c r="B28" s="239"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="240"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -14712,7 +14834,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -14731,40 +14853,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>888</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
-      <c r="G1" s="232"/>
-      <c r="H1" s="233"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="233"/>
+      <c r="H1" s="234"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="243"/>
-      <c r="B2" s="244"/>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="245"/>
+      <c r="A2" s="244"/>
+      <c r="B2" s="245"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="246"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="246" t="s">
+      <c r="A3" s="247" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="247"/>
-      <c r="C3" s="248"/>
-      <c r="D3" s="249"/>
-      <c r="E3" s="246" t="s">
+      <c r="B3" s="248"/>
+      <c r="C3" s="249"/>
+      <c r="D3" s="250"/>
+      <c r="E3" s="247" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="247"/>
-      <c r="G3" s="248"/>
-      <c r="H3" s="249"/>
+      <c r="F3" s="248"/>
+      <c r="G3" s="249"/>
+      <c r="H3" s="250"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="73">
@@ -15432,6 +15554,7 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15439,8 +15562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -15457,40 +15580,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="267" t="s">
+      <c r="A1" s="268" t="s">
         <v>887</v>
       </c>
-      <c r="B1" s="267"/>
-      <c r="C1" s="267"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="267"/>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
+      <c r="B1" s="268"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="268"/>
-      <c r="B2" s="268"/>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
-      <c r="H2" s="268"/>
+      <c r="A2" s="269"/>
+      <c r="B2" s="269"/>
+      <c r="C2" s="269"/>
+      <c r="D2" s="269"/>
+      <c r="E2" s="269"/>
+      <c r="F2" s="269"/>
+      <c r="G2" s="269"/>
+      <c r="H2" s="269"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="269" t="s">
+      <c r="A3" s="270" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="270"/>
-      <c r="C3" s="271"/>
-      <c r="D3" s="272"/>
-      <c r="E3" s="269" t="s">
+      <c r="B3" s="271"/>
+      <c r="C3" s="272"/>
+      <c r="D3" s="273"/>
+      <c r="E3" s="270" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="270"/>
-      <c r="G3" s="271"/>
-      <c r="H3" s="272"/>
+      <c r="F3" s="271"/>
+      <c r="G3" s="272"/>
+      <c r="H3" s="273"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="124">
@@ -16019,36 +16142,36 @@
       <c r="H24" s="152"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="269" t="s">
+      <c r="A25" s="270" t="s">
         <v>772</v>
       </c>
-      <c r="B25" s="270"/>
-      <c r="C25" s="271"/>
-      <c r="D25" s="272"/>
-      <c r="E25" s="269" t="s">
+      <c r="B25" s="271"/>
+      <c r="C25" s="272"/>
+      <c r="D25" s="273"/>
+      <c r="E25" s="270" t="s">
         <v>773</v>
       </c>
-      <c r="F25" s="270"/>
-      <c r="G25" s="271"/>
-      <c r="H25" s="272"/>
+      <c r="F25" s="271"/>
+      <c r="G25" s="272"/>
+      <c r="H25" s="273"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="128" t="s">
         <v>774</v>
       </c>
-      <c r="B26" s="256" t="s">
+      <c r="B26" s="257" t="s">
         <v>775</v>
       </c>
-      <c r="C26" s="257"/>
-      <c r="D26" s="258"/>
+      <c r="C26" s="258"/>
+      <c r="D26" s="259"/>
       <c r="E26" s="124" t="s">
         <v>776</v>
       </c>
-      <c r="F26" s="264" t="s">
+      <c r="F26" s="265" t="s">
         <v>777</v>
       </c>
-      <c r="G26" s="265"/>
-      <c r="H26" s="266" t="s">
+      <c r="G26" s="266"/>
+      <c r="H26" s="267" t="s">
         <v>747</v>
       </c>
     </row>
@@ -16056,21 +16179,21 @@
       <c r="A27" s="136" t="s">
         <v>778</v>
       </c>
-      <c r="B27" s="259" t="s">
+      <c r="B27" s="260" t="s">
         <v>779</v>
       </c>
-      <c r="C27" s="260"/>
-      <c r="D27" s="262" t="s">
+      <c r="C27" s="261"/>
+      <c r="D27" s="263" t="s">
         <v>621</v>
       </c>
       <c r="E27" s="128" t="s">
         <v>780</v>
       </c>
-      <c r="F27" s="256" t="s">
+      <c r="F27" s="257" t="s">
         <v>781</v>
       </c>
-      <c r="G27" s="257"/>
-      <c r="H27" s="263" t="s">
+      <c r="G27" s="258"/>
+      <c r="H27" s="264" t="s">
         <v>749</v>
       </c>
     </row>
@@ -16078,21 +16201,21 @@
       <c r="A28" s="128" t="s">
         <v>782</v>
       </c>
-      <c r="B28" s="256" t="s">
+      <c r="B28" s="257" t="s">
         <v>783</v>
       </c>
-      <c r="C28" s="257"/>
-      <c r="D28" s="258" t="s">
+      <c r="C28" s="258"/>
+      <c r="D28" s="259" t="s">
         <v>622</v>
       </c>
       <c r="E28" s="136" t="s">
         <v>784</v>
       </c>
-      <c r="F28" s="259" t="s">
+      <c r="F28" s="260" t="s">
         <v>785</v>
       </c>
-      <c r="G28" s="260"/>
-      <c r="H28" s="261" t="s">
+      <c r="G28" s="261"/>
+      <c r="H28" s="262" t="s">
         <v>751</v>
       </c>
     </row>
@@ -16100,21 +16223,21 @@
       <c r="A29" s="136" t="s">
         <v>786</v>
       </c>
-      <c r="B29" s="259" t="s">
+      <c r="B29" s="260" t="s">
         <v>787</v>
       </c>
-      <c r="C29" s="260"/>
-      <c r="D29" s="262" t="s">
+      <c r="C29" s="261"/>
+      <c r="D29" s="263" t="s">
         <v>623</v>
       </c>
       <c r="E29" s="128" t="s">
         <v>788</v>
       </c>
-      <c r="F29" s="256" t="s">
+      <c r="F29" s="257" t="s">
         <v>789</v>
       </c>
-      <c r="G29" s="257"/>
-      <c r="H29" s="263" t="s">
+      <c r="G29" s="258"/>
+      <c r="H29" s="264" t="s">
         <v>753</v>
       </c>
     </row>
@@ -16122,21 +16245,21 @@
       <c r="A30" s="128" t="s">
         <v>790</v>
       </c>
-      <c r="B30" s="256" t="s">
+      <c r="B30" s="257" t="s">
         <v>791</v>
       </c>
-      <c r="C30" s="257"/>
-      <c r="D30" s="258" t="s">
+      <c r="C30" s="258"/>
+      <c r="D30" s="259" t="s">
         <v>624</v>
       </c>
       <c r="E30" s="136" t="s">
         <v>792</v>
       </c>
-      <c r="F30" s="259" t="s">
+      <c r="F30" s="260" t="s">
         <v>793</v>
       </c>
-      <c r="G30" s="260"/>
-      <c r="H30" s="261" t="s">
+      <c r="G30" s="261"/>
+      <c r="H30" s="262" t="s">
         <v>755</v>
       </c>
     </row>
@@ -16144,21 +16267,21 @@
       <c r="A31" s="136" t="s">
         <v>794</v>
       </c>
-      <c r="B31" s="259" t="s">
+      <c r="B31" s="260" t="s">
         <v>795</v>
       </c>
-      <c r="C31" s="260"/>
-      <c r="D31" s="262" t="s">
+      <c r="C31" s="261"/>
+      <c r="D31" s="263" t="s">
         <v>625</v>
       </c>
       <c r="E31" s="128" t="s">
         <v>796</v>
       </c>
-      <c r="F31" s="256" t="s">
+      <c r="F31" s="257" t="s">
         <v>797</v>
       </c>
-      <c r="G31" s="257"/>
-      <c r="H31" s="263" t="s">
+      <c r="G31" s="258"/>
+      <c r="H31" s="264" t="s">
         <v>494</v>
       </c>
     </row>
@@ -16166,17 +16289,17 @@
       <c r="A32" s="128" t="s">
         <v>798</v>
       </c>
-      <c r="B32" s="256" t="s">
+      <c r="B32" s="257" t="s">
         <v>799</v>
       </c>
-      <c r="C32" s="257"/>
-      <c r="D32" s="258" t="s">
+      <c r="C32" s="258"/>
+      <c r="D32" s="259" t="s">
         <v>626</v>
       </c>
       <c r="E32" s="136"/>
-      <c r="F32" s="259"/>
-      <c r="G32" s="260"/>
-      <c r="H32" s="261" t="s">
+      <c r="F32" s="260"/>
+      <c r="G32" s="261"/>
+      <c r="H32" s="262" t="s">
         <v>495</v>
       </c>
     </row>
@@ -16184,17 +16307,17 @@
       <c r="A33" s="136" t="s">
         <v>800</v>
       </c>
-      <c r="B33" s="259" t="s">
+      <c r="B33" s="260" t="s">
         <v>801</v>
       </c>
-      <c r="C33" s="260"/>
-      <c r="D33" s="262" t="s">
+      <c r="C33" s="261"/>
+      <c r="D33" s="263" t="s">
         <v>620</v>
       </c>
       <c r="E33" s="128"/>
-      <c r="F33" s="256"/>
-      <c r="G33" s="257"/>
-      <c r="H33" s="263" t="s">
+      <c r="F33" s="257"/>
+      <c r="G33" s="258"/>
+      <c r="H33" s="264" t="s">
         <v>747</v>
       </c>
     </row>
@@ -16202,17 +16325,17 @@
       <c r="A34" s="128" t="s">
         <v>802</v>
       </c>
-      <c r="B34" s="256" t="s">
+      <c r="B34" s="257" t="s">
         <v>803</v>
       </c>
-      <c r="C34" s="257"/>
-      <c r="D34" s="258" t="s">
+      <c r="C34" s="258"/>
+      <c r="D34" s="259" t="s">
         <v>621</v>
       </c>
       <c r="E34" s="136"/>
-      <c r="F34" s="259"/>
-      <c r="G34" s="260"/>
-      <c r="H34" s="261" t="s">
+      <c r="F34" s="260"/>
+      <c r="G34" s="261"/>
+      <c r="H34" s="262" t="s">
         <v>749</v>
       </c>
     </row>
@@ -16220,17 +16343,17 @@
       <c r="A35" s="136" t="s">
         <v>804</v>
       </c>
-      <c r="B35" s="259" t="s">
+      <c r="B35" s="260" t="s">
         <v>805</v>
       </c>
-      <c r="C35" s="260"/>
-      <c r="D35" s="262" t="s">
+      <c r="C35" s="261"/>
+      <c r="D35" s="263" t="s">
         <v>622</v>
       </c>
       <c r="E35" s="128"/>
-      <c r="F35" s="256"/>
-      <c r="G35" s="257"/>
-      <c r="H35" s="263" t="s">
+      <c r="F35" s="257"/>
+      <c r="G35" s="258"/>
+      <c r="H35" s="264" t="s">
         <v>751</v>
       </c>
     </row>
@@ -16238,17 +16361,17 @@
       <c r="A36" s="128" t="s">
         <v>806</v>
       </c>
-      <c r="B36" s="256" t="s">
+      <c r="B36" s="257" t="s">
         <v>807</v>
       </c>
-      <c r="C36" s="257"/>
-      <c r="D36" s="258" t="s">
+      <c r="C36" s="258"/>
+      <c r="D36" s="259" t="s">
         <v>623</v>
       </c>
       <c r="E36" s="136"/>
-      <c r="F36" s="259"/>
-      <c r="G36" s="260"/>
-      <c r="H36" s="261" t="s">
+      <c r="F36" s="260"/>
+      <c r="G36" s="261"/>
+      <c r="H36" s="262" t="s">
         <v>753</v>
       </c>
     </row>
@@ -16256,17 +16379,17 @@
       <c r="A37" s="136" t="s">
         <v>808</v>
       </c>
-      <c r="B37" s="259" t="s">
+      <c r="B37" s="260" t="s">
         <v>809</v>
       </c>
-      <c r="C37" s="260"/>
-      <c r="D37" s="262" t="s">
+      <c r="C37" s="261"/>
+      <c r="D37" s="263" t="s">
         <v>624</v>
       </c>
       <c r="E37" s="128"/>
-      <c r="F37" s="256"/>
-      <c r="G37" s="257"/>
-      <c r="H37" s="263" t="s">
+      <c r="F37" s="257"/>
+      <c r="G37" s="258"/>
+      <c r="H37" s="264" t="s">
         <v>755</v>
       </c>
     </row>
@@ -16274,17 +16397,17 @@
       <c r="A38" s="128" t="s">
         <v>810</v>
       </c>
-      <c r="B38" s="256" t="s">
+      <c r="B38" s="257" t="s">
         <v>811</v>
       </c>
-      <c r="C38" s="257"/>
-      <c r="D38" s="258" t="s">
+      <c r="C38" s="258"/>
+      <c r="D38" s="259" t="s">
         <v>625</v>
       </c>
       <c r="E38" s="136"/>
-      <c r="F38" s="259"/>
-      <c r="G38" s="260"/>
-      <c r="H38" s="261" t="s">
+      <c r="F38" s="260"/>
+      <c r="G38" s="261"/>
+      <c r="H38" s="262" t="s">
         <v>494</v>
       </c>
     </row>
@@ -16292,17 +16415,17 @@
       <c r="A39" s="136" t="s">
         <v>812</v>
       </c>
-      <c r="B39" s="259" t="s">
+      <c r="B39" s="260" t="s">
         <v>813</v>
       </c>
-      <c r="C39" s="260"/>
-      <c r="D39" s="262" t="s">
+      <c r="C39" s="261"/>
+      <c r="D39" s="263" t="s">
         <v>626</v>
       </c>
       <c r="E39" s="128"/>
-      <c r="F39" s="256"/>
-      <c r="G39" s="257"/>
-      <c r="H39" s="263" t="s">
+      <c r="F39" s="257"/>
+      <c r="G39" s="258"/>
+      <c r="H39" s="264" t="s">
         <v>495</v>
       </c>
     </row>
@@ -16310,33 +16433,33 @@
       <c r="A40" s="128" t="s">
         <v>814</v>
       </c>
-      <c r="B40" s="256" t="s">
+      <c r="B40" s="257" t="s">
         <v>813</v>
       </c>
-      <c r="C40" s="257"/>
-      <c r="D40" s="258" t="s">
+      <c r="C40" s="258"/>
+      <c r="D40" s="259" t="s">
         <v>626</v>
       </c>
       <c r="E40" s="136"/>
-      <c r="F40" s="259"/>
-      <c r="G40" s="260"/>
-      <c r="H40" s="261"/>
+      <c r="F40" s="260"/>
+      <c r="G40" s="261"/>
+      <c r="H40" s="262"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="148" t="s">
         <v>815</v>
       </c>
-      <c r="B41" s="250" t="s">
+      <c r="B41" s="251" t="s">
         <v>813</v>
       </c>
-      <c r="C41" s="251"/>
-      <c r="D41" s="252" t="s">
+      <c r="C41" s="252"/>
+      <c r="D41" s="253" t="s">
         <v>626</v>
       </c>
       <c r="E41" s="153"/>
-      <c r="F41" s="253"/>
-      <c r="G41" s="254"/>
-      <c r="H41" s="255"/>
+      <c r="F41" s="254"/>
+      <c r="G41" s="255"/>
+      <c r="H41" s="256"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -16380,5 +16503,6 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>